<commit_message>
fix simple in INSPARCHARACTERISTIC
</commit_message>
<xml_diff>
--- a/resource/Dict/unit.XLSX
+++ b/resource/Dict/unit.XLSX
@@ -7,17 +7,19 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Unit" sheetId="1" r:id="rId1"/>
+    <sheet name="Sampling" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sampling!$A$1:$B$255</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unit!$A$1:$G$501</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="1512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3516" uniqueCount="1936">
   <si>
     <t>EN</t>
   </si>
@@ -4553,16 +4555,1293 @@
   </si>
   <si>
     <t>Measurement unit text</t>
+  </si>
+  <si>
+    <t>FF1</t>
+  </si>
+  <si>
+    <t>FHF0N1</t>
+  </si>
+  <si>
+    <t>FF2</t>
+  </si>
+  <si>
+    <t>FHF0N2</t>
+  </si>
+  <si>
+    <t>FF3</t>
+  </si>
+  <si>
+    <t>FHF0N3</t>
+  </si>
+  <si>
+    <t>FF4</t>
+  </si>
+  <si>
+    <t>FHF0N4</t>
+  </si>
+  <si>
+    <t>FF5</t>
+  </si>
+  <si>
+    <t>FHF0N5</t>
+  </si>
+  <si>
+    <t>FF6</t>
+  </si>
+  <si>
+    <t>FHF0N6</t>
+  </si>
+  <si>
+    <t>FF7</t>
+  </si>
+  <si>
+    <t>FHF0N7</t>
+  </si>
+  <si>
+    <t>FF8</t>
+  </si>
+  <si>
+    <t>FHF0N8</t>
+  </si>
+  <si>
+    <t>FF9</t>
+  </si>
+  <si>
+    <t>FHF0N9</t>
+  </si>
+  <si>
+    <t>FF10</t>
+  </si>
+  <si>
+    <t>FHF0N10</t>
+  </si>
+  <si>
+    <t>FF11</t>
+  </si>
+  <si>
+    <t>FHF0N11</t>
+  </si>
+  <si>
+    <t>FF12</t>
+  </si>
+  <si>
+    <t>FHF0N12</t>
+  </si>
+  <si>
+    <t>FF13</t>
+  </si>
+  <si>
+    <t>FHF0N13</t>
+  </si>
+  <si>
+    <t>FF14</t>
+  </si>
+  <si>
+    <t>FHF0N14</t>
+  </si>
+  <si>
+    <t>FF15</t>
+  </si>
+  <si>
+    <t>FHF0N15</t>
+  </si>
+  <si>
+    <t>FF16</t>
+  </si>
+  <si>
+    <t>FHF0N16</t>
+  </si>
+  <si>
+    <t>FF17</t>
+  </si>
+  <si>
+    <t>FHF0N17</t>
+  </si>
+  <si>
+    <t>FF18</t>
+  </si>
+  <si>
+    <t>FHF0N18</t>
+  </si>
+  <si>
+    <t>FF19</t>
+  </si>
+  <si>
+    <t>FHF0N19</t>
+  </si>
+  <si>
+    <t>FF20</t>
+  </si>
+  <si>
+    <t>FHF0N20</t>
+  </si>
+  <si>
+    <t>FF25</t>
+  </si>
+  <si>
+    <t>FHF0N25</t>
+  </si>
+  <si>
+    <t>FF30</t>
+  </si>
+  <si>
+    <t>FHF0N30</t>
+  </si>
+  <si>
+    <t>FF31</t>
+  </si>
+  <si>
+    <t>FHF0N31</t>
+  </si>
+  <si>
+    <t>FF32</t>
+  </si>
+  <si>
+    <t>FHF0N32</t>
+  </si>
+  <si>
+    <t>FF33</t>
+  </si>
+  <si>
+    <t>FHF0N33</t>
+  </si>
+  <si>
+    <t>FF34</t>
+  </si>
+  <si>
+    <t>FHF0N34</t>
+  </si>
+  <si>
+    <t>FF35</t>
+  </si>
+  <si>
+    <t>FHF0N35</t>
+  </si>
+  <si>
+    <t>FF40</t>
+  </si>
+  <si>
+    <t>FHF0N40</t>
+  </si>
+  <si>
+    <t>FF48</t>
+  </si>
+  <si>
+    <t>FHF0N48</t>
+  </si>
+  <si>
+    <t>FF50</t>
+  </si>
+  <si>
+    <t>FHF0N50</t>
+  </si>
+  <si>
+    <t>FF60</t>
+  </si>
+  <si>
+    <t>FHF0N60</t>
+  </si>
+  <si>
+    <t>FF80</t>
+  </si>
+  <si>
+    <t>FHF0N80</t>
+  </si>
+  <si>
+    <t>FF100</t>
+  </si>
+  <si>
+    <t>FHF0N100</t>
+  </si>
+  <si>
+    <t>FF125</t>
+  </si>
+  <si>
+    <t>FHF0N125</t>
+  </si>
+  <si>
+    <t>FF150</t>
+  </si>
+  <si>
+    <t>FHF0N150</t>
+  </si>
+  <si>
+    <t>FF200</t>
+  </si>
+  <si>
+    <t>FHF0N200</t>
+  </si>
+  <si>
+    <t>FF250</t>
+  </si>
+  <si>
+    <t>FHF0N250</t>
+  </si>
+  <si>
+    <t>FF315</t>
+  </si>
+  <si>
+    <t>FHF0N315</t>
+  </si>
+  <si>
+    <t>FF500</t>
+  </si>
+  <si>
+    <t>FHF0N500</t>
+  </si>
+  <si>
+    <t>FF800</t>
+  </si>
+  <si>
+    <t>FHF0N800</t>
+  </si>
+  <si>
+    <t>FF1250</t>
+  </si>
+  <si>
+    <t>FP1</t>
+  </si>
+  <si>
+    <t>FHP0N1</t>
+  </si>
+  <si>
+    <t>FP2</t>
+  </si>
+  <si>
+    <t>FHP0N2</t>
+  </si>
+  <si>
+    <t>FP3</t>
+  </si>
+  <si>
+    <t>FHP0N3</t>
+  </si>
+  <si>
+    <t>FP4</t>
+  </si>
+  <si>
+    <t>FHP0N4</t>
+  </si>
+  <si>
+    <t>FP5</t>
+  </si>
+  <si>
+    <t>FHP0N5</t>
+  </si>
+  <si>
+    <t>FP6</t>
+  </si>
+  <si>
+    <t>FHP0N6</t>
+  </si>
+  <si>
+    <t>FP7</t>
+  </si>
+  <si>
+    <t>FHP0N7</t>
+  </si>
+  <si>
+    <t>FP8</t>
+  </si>
+  <si>
+    <t>FHP0N8</t>
+  </si>
+  <si>
+    <t>FP9</t>
+  </si>
+  <si>
+    <t>FHP0N9</t>
+  </si>
+  <si>
+    <t>FP10</t>
+  </si>
+  <si>
+    <t>FHP0N10</t>
+  </si>
+  <si>
+    <t>FP15</t>
+  </si>
+  <si>
+    <t>FHP0N15</t>
+  </si>
+  <si>
+    <t>FP20</t>
+  </si>
+  <si>
+    <t>FHP0N20</t>
+  </si>
+  <si>
+    <t>FP25</t>
+  </si>
+  <si>
+    <t>FHP0N25</t>
+  </si>
+  <si>
+    <t>FP30</t>
+  </si>
+  <si>
+    <t>FHP0N30</t>
+  </si>
+  <si>
+    <t>FP40</t>
+  </si>
+  <si>
+    <t>FHP0N40</t>
+  </si>
+  <si>
+    <t>FP50</t>
+  </si>
+  <si>
+    <t>FHP0N50</t>
+  </si>
+  <si>
+    <t>FP60</t>
+  </si>
+  <si>
+    <t>FHP0N60</t>
+  </si>
+  <si>
+    <t>FP70</t>
+  </si>
+  <si>
+    <t>FHP0N70</t>
+  </si>
+  <si>
+    <t>FP80</t>
+  </si>
+  <si>
+    <t>FHP0N80</t>
+  </si>
+  <si>
+    <t>FP90</t>
+  </si>
+  <si>
+    <t>FHP0N90</t>
+  </si>
+  <si>
+    <t>FP100</t>
+  </si>
+  <si>
+    <t>FHP0N100</t>
+  </si>
+  <si>
+    <t>FSI0.01</t>
+  </si>
+  <si>
+    <t>FSI1.5</t>
+  </si>
+  <si>
+    <t>FSI2.5</t>
+  </si>
+  <si>
+    <t>FSI4</t>
+  </si>
+  <si>
+    <t>FSI10</t>
+  </si>
+  <si>
+    <t>FSII0.01</t>
+  </si>
+  <si>
+    <t>FSII1</t>
+  </si>
+  <si>
+    <t>FSII1.5</t>
+  </si>
+  <si>
+    <t>FSII2.5</t>
+  </si>
+  <si>
+    <t>FSII4</t>
+  </si>
+  <si>
+    <t>FSII10</t>
+  </si>
+  <si>
+    <t>FSIII.01</t>
+  </si>
+  <si>
+    <t>FSIII1.5</t>
+  </si>
+  <si>
+    <t>FSS10.01</t>
+  </si>
+  <si>
+    <t>FSS20.01</t>
+  </si>
+  <si>
+    <t>FSS20.65</t>
+  </si>
+  <si>
+    <t>FSS21</t>
+  </si>
+  <si>
+    <t>FSS21.5</t>
+  </si>
+  <si>
+    <t>FSS22.5</t>
+  </si>
+  <si>
+    <t>FSS24</t>
+  </si>
+  <si>
+    <t>FSS30.01</t>
+  </si>
+  <si>
+    <t>FSS31</t>
+  </si>
+  <si>
+    <t>FSS31.5</t>
+  </si>
+  <si>
+    <t>FSS32.5</t>
+  </si>
+  <si>
+    <t>FSS40.01</t>
+  </si>
+  <si>
+    <t>FSS41</t>
+  </si>
+  <si>
+    <t>FMI0.65</t>
+  </si>
+  <si>
+    <t>FMI1.5</t>
+  </si>
+  <si>
+    <t>FMI4</t>
+  </si>
+  <si>
+    <t>FMI10</t>
+  </si>
+  <si>
+    <t>FMII0.65</t>
+  </si>
+  <si>
+    <t>FMII2.5</t>
+  </si>
+  <si>
+    <t>FMS10.01</t>
+  </si>
+  <si>
+    <t>FMS11.5</t>
+  </si>
+  <si>
+    <t>FMS14</t>
+  </si>
+  <si>
+    <t>FMS20.01</t>
+  </si>
+  <si>
+    <t>FMS21</t>
+  </si>
+  <si>
+    <t>FMS24</t>
+  </si>
+  <si>
+    <t>FMS30.01</t>
+  </si>
+  <si>
+    <t>FMS31.5</t>
+  </si>
+  <si>
+    <t>FMS34</t>
+  </si>
+  <si>
+    <t>FMS310</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>FPF1</t>
+  </si>
+  <si>
+    <t>FHF1N1</t>
+  </si>
+  <si>
+    <t>FPF2</t>
+  </si>
+  <si>
+    <t>FHF1N2</t>
+  </si>
+  <si>
+    <t>FPF3</t>
+  </si>
+  <si>
+    <t>FHF1N3</t>
+  </si>
+  <si>
+    <t>FPF4</t>
+  </si>
+  <si>
+    <t>FHF1N4</t>
+  </si>
+  <si>
+    <t>FPF5</t>
+  </si>
+  <si>
+    <t>FHF1N5</t>
+  </si>
+  <si>
+    <t>FPF6</t>
+  </si>
+  <si>
+    <t>FHF1N6</t>
+  </si>
+  <si>
+    <t>FPF7</t>
+  </si>
+  <si>
+    <t>FHF1N7</t>
+  </si>
+  <si>
+    <t>FPF8</t>
+  </si>
+  <si>
+    <t>FHF1N8</t>
+  </si>
+  <si>
+    <t>FPF9</t>
+  </si>
+  <si>
+    <t>FHF1N9</t>
+  </si>
+  <si>
+    <t>FPF10</t>
+  </si>
+  <si>
+    <t>FHF1N10</t>
+  </si>
+  <si>
+    <t>FPF11</t>
+  </si>
+  <si>
+    <t>FHF1N11</t>
+  </si>
+  <si>
+    <t>FPF12</t>
+  </si>
+  <si>
+    <t>FHF1N12</t>
+  </si>
+  <si>
+    <t>FPF13</t>
+  </si>
+  <si>
+    <t>FHF1N13</t>
+  </si>
+  <si>
+    <t>FPF14</t>
+  </si>
+  <si>
+    <t>FHF1N14</t>
+  </si>
+  <si>
+    <t>FPF15</t>
+  </si>
+  <si>
+    <t>FHF1N15</t>
+  </si>
+  <si>
+    <t>FPF16</t>
+  </si>
+  <si>
+    <t>FHF1N16</t>
+  </si>
+  <si>
+    <t>FPF17</t>
+  </si>
+  <si>
+    <t>FHF1N17</t>
+  </si>
+  <si>
+    <t>FPF18</t>
+  </si>
+  <si>
+    <t>FHF1N18</t>
+  </si>
+  <si>
+    <t>FPF19</t>
+  </si>
+  <si>
+    <t>FHF1N19</t>
+  </si>
+  <si>
+    <t>FPF20</t>
+  </si>
+  <si>
+    <t>FHF1N20</t>
+  </si>
+  <si>
+    <t>FPF25</t>
+  </si>
+  <si>
+    <t>FHF1N25</t>
+  </si>
+  <si>
+    <t>FPF30</t>
+  </si>
+  <si>
+    <t>FHF1N30</t>
+  </si>
+  <si>
+    <t>FPF31</t>
+  </si>
+  <si>
+    <t>FHF1N31</t>
+  </si>
+  <si>
+    <t>FPF32</t>
+  </si>
+  <si>
+    <t>FHF1N32</t>
+  </si>
+  <si>
+    <t>FPF33</t>
+  </si>
+  <si>
+    <t>FHF1N33</t>
+  </si>
+  <si>
+    <t>FPF34</t>
+  </si>
+  <si>
+    <t>FHF1N34</t>
+  </si>
+  <si>
+    <t>FPF35</t>
+  </si>
+  <si>
+    <t>FHF1N35</t>
+  </si>
+  <si>
+    <t>FPF40</t>
+  </si>
+  <si>
+    <t>FHF1N40</t>
+  </si>
+  <si>
+    <t>FPF48</t>
+  </si>
+  <si>
+    <t>FHF1N48</t>
+  </si>
+  <si>
+    <t>FPF50</t>
+  </si>
+  <si>
+    <t>FHF1N50</t>
+  </si>
+  <si>
+    <t>FPF60</t>
+  </si>
+  <si>
+    <t>FHF1N60</t>
+  </si>
+  <si>
+    <t>FPF80</t>
+  </si>
+  <si>
+    <t>FHF1N80</t>
+  </si>
+  <si>
+    <t>FPF100</t>
+  </si>
+  <si>
+    <t>FHF1N100</t>
+  </si>
+  <si>
+    <t>FPF125</t>
+  </si>
+  <si>
+    <t>FHF1N125</t>
+  </si>
+  <si>
+    <t>FPF150</t>
+  </si>
+  <si>
+    <t>FHF1N150</t>
+  </si>
+  <si>
+    <t>FPF200</t>
+  </si>
+  <si>
+    <t>FHF1N200</t>
+  </si>
+  <si>
+    <t>FPF250</t>
+  </si>
+  <si>
+    <t>FHF1N250</t>
+  </si>
+  <si>
+    <t>FPF315</t>
+  </si>
+  <si>
+    <t>FHF1N315</t>
+  </si>
+  <si>
+    <t>FPF500</t>
+  </si>
+  <si>
+    <t>FHF1N500</t>
+  </si>
+  <si>
+    <t>FPF800</t>
+  </si>
+  <si>
+    <t>FHF1N800</t>
+  </si>
+  <si>
+    <t>FPF1250</t>
+  </si>
+  <si>
+    <t>FPP1</t>
+  </si>
+  <si>
+    <t>FHP1N1</t>
+  </si>
+  <si>
+    <t>FPP2</t>
+  </si>
+  <si>
+    <t>FHP1N2</t>
+  </si>
+  <si>
+    <t>FPP3</t>
+  </si>
+  <si>
+    <t>FHP1N3</t>
+  </si>
+  <si>
+    <t>FPP4</t>
+  </si>
+  <si>
+    <t>FHP1N4</t>
+  </si>
+  <si>
+    <t>FPP5</t>
+  </si>
+  <si>
+    <t>FHP1N5</t>
+  </si>
+  <si>
+    <t>FPP6</t>
+  </si>
+  <si>
+    <t>FHP1N6</t>
+  </si>
+  <si>
+    <t>FPP7</t>
+  </si>
+  <si>
+    <t>FHP1N7</t>
+  </si>
+  <si>
+    <t>FPP8</t>
+  </si>
+  <si>
+    <t>FHP1N8</t>
+  </si>
+  <si>
+    <t>FPP9</t>
+  </si>
+  <si>
+    <t>FHP1N9</t>
+  </si>
+  <si>
+    <t>FPP10</t>
+  </si>
+  <si>
+    <t>FHP1N10</t>
+  </si>
+  <si>
+    <t>FPP15</t>
+  </si>
+  <si>
+    <t>FHP1N15</t>
+  </si>
+  <si>
+    <t>FPP20</t>
+  </si>
+  <si>
+    <t>FHP1N20</t>
+  </si>
+  <si>
+    <t>FPP25</t>
+  </si>
+  <si>
+    <t>FHP1N25</t>
+  </si>
+  <si>
+    <t>FPP30</t>
+  </si>
+  <si>
+    <t>FHP1N30</t>
+  </si>
+  <si>
+    <t>FPP40</t>
+  </si>
+  <si>
+    <t>FHP1N40</t>
+  </si>
+  <si>
+    <t>FPP50</t>
+  </si>
+  <si>
+    <t>FHP1N50</t>
+  </si>
+  <si>
+    <t>FPP60</t>
+  </si>
+  <si>
+    <t>FHP1N60</t>
+  </si>
+  <si>
+    <t>FPP70</t>
+  </si>
+  <si>
+    <t>FHP1N70</t>
+  </si>
+  <si>
+    <t>FPP80</t>
+  </si>
+  <si>
+    <t>FHP1N80</t>
+  </si>
+  <si>
+    <t>FPP90</t>
+  </si>
+  <si>
+    <t>FHP1N90</t>
+  </si>
+  <si>
+    <t>FPP100</t>
+  </si>
+  <si>
+    <t>FHP1N100</t>
+  </si>
+  <si>
+    <t>FPSI0.01</t>
+  </si>
+  <si>
+    <t>FPSI1.5</t>
+  </si>
+  <si>
+    <t>FPSI2.5</t>
+  </si>
+  <si>
+    <t>FPSI4</t>
+  </si>
+  <si>
+    <t>FPSI10</t>
+  </si>
+  <si>
+    <t>FPSII.01</t>
+  </si>
+  <si>
+    <t>FPSII1</t>
+  </si>
+  <si>
+    <t>FPSII1.5</t>
+  </si>
+  <si>
+    <t>FPSII2.5</t>
+  </si>
+  <si>
+    <t>FPSII4</t>
+  </si>
+  <si>
+    <t>FPSII10</t>
+  </si>
+  <si>
+    <t>FPS3.01</t>
+  </si>
+  <si>
+    <t>FPS3 1.5</t>
+  </si>
+  <si>
+    <t>FPSS1.01</t>
+  </si>
+  <si>
+    <t>FPSS2.01</t>
+  </si>
+  <si>
+    <t>FPSS2.65</t>
+  </si>
+  <si>
+    <t>FPSS21</t>
+  </si>
+  <si>
+    <t>FPSS21.5</t>
+  </si>
+  <si>
+    <t>FPSS22.5</t>
+  </si>
+  <si>
+    <t>FPSS24</t>
+  </si>
+  <si>
+    <t>FPSS3.01</t>
+  </si>
+  <si>
+    <t>FPSS31</t>
+  </si>
+  <si>
+    <t>FPSS31.5</t>
+  </si>
+  <si>
+    <t>FPSS32.5</t>
+  </si>
+  <si>
+    <t>FPSS4.01</t>
+  </si>
+  <si>
+    <t>FPSS41</t>
+  </si>
+  <si>
+    <t>FPMI0.65</t>
+  </si>
+  <si>
+    <t>FPMI1.5</t>
+  </si>
+  <si>
+    <t>FPMI4</t>
+  </si>
+  <si>
+    <t>FPMI10</t>
+  </si>
+  <si>
+    <t>FPMII.65</t>
+  </si>
+  <si>
+    <t>FPMII2.5</t>
+  </si>
+  <si>
+    <t>FPMS1.01</t>
+  </si>
+  <si>
+    <t>FPMS11.5</t>
+  </si>
+  <si>
+    <t>FPMS14</t>
+  </si>
+  <si>
+    <t>FPMS2.01</t>
+  </si>
+  <si>
+    <t>FPMS21</t>
+  </si>
+  <si>
+    <t>FPMS24</t>
+  </si>
+  <si>
+    <t>FPMS3.01</t>
+  </si>
+  <si>
+    <t>FPMS31.5</t>
+  </si>
+  <si>
+    <t>FPMS34</t>
+  </si>
+  <si>
+    <t>FPMS310</t>
+  </si>
+  <si>
+    <t>FSF1</t>
+  </si>
+  <si>
+    <t>FHF0S1</t>
+  </si>
+  <si>
+    <t>FSF2</t>
+  </si>
+  <si>
+    <t>FHF0S2</t>
+  </si>
+  <si>
+    <t>FSF3</t>
+  </si>
+  <si>
+    <t>FHF0S3</t>
+  </si>
+  <si>
+    <t>FSF4</t>
+  </si>
+  <si>
+    <t>FHF0S4</t>
+  </si>
+  <si>
+    <t>FSF5</t>
+  </si>
+  <si>
+    <t>FHF0S5</t>
+  </si>
+  <si>
+    <t>FSF6</t>
+  </si>
+  <si>
+    <t>FHF0S6</t>
+  </si>
+  <si>
+    <t>FSF7</t>
+  </si>
+  <si>
+    <t>FHF0S7</t>
+  </si>
+  <si>
+    <t>FSF8</t>
+  </si>
+  <si>
+    <t>FHF0S8</t>
+  </si>
+  <si>
+    <t>FSF9</t>
+  </si>
+  <si>
+    <t>FHF0S9</t>
+  </si>
+  <si>
+    <t>FSF10</t>
+  </si>
+  <si>
+    <t>FHF0S10</t>
+  </si>
+  <si>
+    <t>FSF11</t>
+  </si>
+  <si>
+    <t>FHF0S11</t>
+  </si>
+  <si>
+    <t>FSF12</t>
+  </si>
+  <si>
+    <t>FHF0S12</t>
+  </si>
+  <si>
+    <t>FSF13</t>
+  </si>
+  <si>
+    <t>FHF0S13</t>
+  </si>
+  <si>
+    <t>FSF14</t>
+  </si>
+  <si>
+    <t>FHF0S14</t>
+  </si>
+  <si>
+    <t>FSF15</t>
+  </si>
+  <si>
+    <t>FHF0S15</t>
+  </si>
+  <si>
+    <t>FSF16</t>
+  </si>
+  <si>
+    <t>FHF0S16</t>
+  </si>
+  <si>
+    <t>FSF17</t>
+  </si>
+  <si>
+    <t>FHF0S17</t>
+  </si>
+  <si>
+    <t>FSF18</t>
+  </si>
+  <si>
+    <t>FHF0S18</t>
+  </si>
+  <si>
+    <t>FSF19</t>
+  </si>
+  <si>
+    <t>FHF0S19</t>
+  </si>
+  <si>
+    <t>FSF20</t>
+  </si>
+  <si>
+    <t>FHF0S20</t>
+  </si>
+  <si>
+    <t>FSF21</t>
+  </si>
+  <si>
+    <t>FHF0S21</t>
+  </si>
+  <si>
+    <t>FSF22</t>
+  </si>
+  <si>
+    <t>FHF0S22</t>
+  </si>
+  <si>
+    <t>FSF23</t>
+  </si>
+  <si>
+    <t>FHF0S23</t>
+  </si>
+  <si>
+    <t>FSPF1</t>
+  </si>
+  <si>
+    <t>FHF1S1</t>
+  </si>
+  <si>
+    <t>FSPF2</t>
+  </si>
+  <si>
+    <t>FHF1S2</t>
+  </si>
+  <si>
+    <t>FSPF3</t>
+  </si>
+  <si>
+    <t>FHF1S3</t>
+  </si>
+  <si>
+    <t>FSPF4</t>
+  </si>
+  <si>
+    <t>FHF1S4</t>
+  </si>
+  <si>
+    <t>FSPF5</t>
+  </si>
+  <si>
+    <t>FHF1S5</t>
+  </si>
+  <si>
+    <t>FSPF6</t>
+  </si>
+  <si>
+    <t>FHF1S6</t>
+  </si>
+  <si>
+    <t>FSPF7</t>
+  </si>
+  <si>
+    <t>FHF1S7</t>
+  </si>
+  <si>
+    <t>FSPF8</t>
+  </si>
+  <si>
+    <t>FHF1S8</t>
+  </si>
+  <si>
+    <t>FSPF9</t>
+  </si>
+  <si>
+    <t>FHF1S9</t>
+  </si>
+  <si>
+    <t>FSPF10</t>
+  </si>
+  <si>
+    <t>FHF1S10</t>
+  </si>
+  <si>
+    <t>FSPF11</t>
+  </si>
+  <si>
+    <t>FHF1S11</t>
+  </si>
+  <si>
+    <t>FSPF12</t>
+  </si>
+  <si>
+    <t>FHF1S12</t>
+  </si>
+  <si>
+    <t>FSPF13</t>
+  </si>
+  <si>
+    <t>FHF1S13</t>
+  </si>
+  <si>
+    <t>FSPF14</t>
+  </si>
+  <si>
+    <t>FHF1S14</t>
+  </si>
+  <si>
+    <t>FSPF15</t>
+  </si>
+  <si>
+    <t>FHF1S15</t>
+  </si>
+  <si>
+    <t>FSPF16</t>
+  </si>
+  <si>
+    <t>FHF1S16</t>
+  </si>
+  <si>
+    <t>FSPF17</t>
+  </si>
+  <si>
+    <t>FHF1S17</t>
+  </si>
+  <si>
+    <t>FSPF18</t>
+  </si>
+  <si>
+    <t>FHF1S18</t>
+  </si>
+  <si>
+    <t>FSPF19</t>
+  </si>
+  <si>
+    <t>FHF1S19</t>
+  </si>
+  <si>
+    <t>FSPF20</t>
+  </si>
+  <si>
+    <t>FHF1S20</t>
+  </si>
+  <si>
+    <t>FSPF21</t>
+  </si>
+  <si>
+    <t>FHF1S21</t>
+  </si>
+  <si>
+    <t>FSPF22</t>
+  </si>
+  <si>
+    <t>FHF1S22</t>
+  </si>
+  <si>
+    <t>FSPF23</t>
+  </si>
+  <si>
+    <t>FHF1S23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -4606,7 +5885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -4615,6 +5894,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4920,7 +6202,7 @@
   <dimension ref="A1:F501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9760,7 +11042,7 @@
       <c r="B242" t="s">
         <v>722</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C242" s="3" t="s">
         <v>722</v>
       </c>
       <c r="D242" t="s">
@@ -14954,9 +16236,2069 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:G501"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B255"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>1607</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>1629</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>1635</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>1637</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>1643</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>1649</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>1651</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>1655</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>1657</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>1658</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>1659</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>1661</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>1663</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B115" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B126" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B127" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B128" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B130" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B131" t="s">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B132" t="s">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B133" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B135" t="s">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B148" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B149" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B153" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B155" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B156" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B159" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B162" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B163" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B164" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B167" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B168" t="s">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B169" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B170" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B171" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B172" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B173" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B174" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B175" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B176" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B177" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B178" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B179" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B180" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B181" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B182" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B183" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B184" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B185" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B186" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B187" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B188" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B189" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B190" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B191" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B192" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B193" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B194" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B195" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B196" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>1831</v>
+      </c>
+      <c r="B197" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B198" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B199" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B200" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>1835</v>
+      </c>
+      <c r="B201" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B202" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B203" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B204" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B205" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B206" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B208" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B209" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B210" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B211" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B212" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B213" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B214" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B215" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B216" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B217" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B218" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B219" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B220" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B221" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B222" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B223" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B224" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>1874</v>
+      </c>
+      <c r="B225" t="s">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B226" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B227" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B228" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B229" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B230" t="s">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B231" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B232" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B233" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B234" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B235" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B236" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>1898</v>
+      </c>
+      <c r="B237" t="s">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B238" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B239" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B240" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B241" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B242" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B243" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B244" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B245" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B246" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B247" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B248" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B249" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B250" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B251" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B252" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B253" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B254" t="s">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B255" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B255"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change MIC Error message
</commit_message>
<xml_diff>
--- a/resource/Dict/unit.XLSX
+++ b/resource/Dict/unit.XLSX
@@ -6201,8 +6201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
+      <selection activeCell="G399" sqref="G399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>